<commit_message>
added more stuff to courses excel doc
</commit_message>
<xml_diff>
--- a/courses.xlsx
+++ b/courses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\gitrepos\CURSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA7C325-BA84-41AA-9580-99B0035014E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DC95F9-D9E1-4037-A8A7-38C1140E10CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1125" windowWidth="43200" windowHeight="22035" xr2:uid="{DDE50F24-E41F-4BD5-849B-5D365588DE5F}"/>
+    <workbookView xWindow="6060" yWindow="2460" windowWidth="28800" windowHeight="14685" xr2:uid="{DDE50F24-E41F-4BD5-849B-5D365588DE5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
   <si>
     <t>Applied Programming Concepts</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>Wayne Bynoe</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Fall</t>
   </si>
 </sst>
 </file>
@@ -444,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441F3BF7-A5CC-4710-AC3E-0C69E492EE1F}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,6 +608,71 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated course excel file
</commit_message>
<xml_diff>
--- a/courses.xlsx
+++ b/courses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\gitrepos\CURSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F1454B-8341-4EF5-B88F-F7D27B9893CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1BDE2C-A1D5-45A8-BFC6-B9DBADA87F69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6120" windowWidth="28800" windowHeight="15435" xr2:uid="{DDE50F24-E41F-4BD5-849B-5D365588DE5F}"/>
+    <workbookView xWindow="3195" yWindow="2880" windowWidth="28800" windowHeight="15435" xr2:uid="{DDE50F24-E41F-4BD5-849B-5D365588DE5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="41">
   <si>
     <t>Applied Programming Concepts</t>
   </si>
@@ -99,6 +99,63 @@
   </si>
   <si>
     <t>Bruce Decker</t>
+  </si>
+  <si>
+    <t>Introduction to Engineering</t>
+  </si>
+  <si>
+    <t>TBA</t>
+  </si>
+  <si>
+    <t>Analog Circuit Design</t>
+  </si>
+  <si>
+    <t>Digital Logic</t>
+  </si>
+  <si>
+    <t>Calc I</t>
+  </si>
+  <si>
+    <t>MATH</t>
+  </si>
+  <si>
+    <t>Mami Wentworth</t>
+  </si>
+  <si>
+    <t>Sociology</t>
+  </si>
+  <si>
+    <t>SOCL</t>
+  </si>
+  <si>
+    <t>Allen Wong</t>
+  </si>
+  <si>
+    <t>Discrete Math</t>
+  </si>
+  <si>
+    <t>Network Theory I</t>
+  </si>
+  <si>
+    <t>Samuel Zeman</t>
+  </si>
+  <si>
+    <t>English II</t>
+  </si>
+  <si>
+    <t>ENGL</t>
+  </si>
+  <si>
+    <t>Hardware Security</t>
+  </si>
+  <si>
+    <t>Lisa Fluet</t>
+  </si>
+  <si>
+    <t>Criminology</t>
+  </si>
+  <si>
+    <t>Calc II</t>
   </si>
 </sst>
 </file>
@@ -456,7 +513,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,63 +698,351 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>12345</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="G7" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="H7" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I7" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>23651</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G8" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="H8" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I8" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>15675</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="G9" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="H9" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I9" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>34865</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G10" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="H10" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>23419</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="G11" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="H11" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I11" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>57438</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G12" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="H12" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I12" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>27329</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="G13" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="H13" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I13" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>34562</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G14" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="H14" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I14" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>38675</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="G15" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="H15" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I15" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>34563</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G16" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45682</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="G17" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>15430</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G18" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="H18" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I18" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>